<commit_message>
Reproduce results from original study. Compare current v. original effects in forest plot
</commit_message>
<xml_diff>
--- a/StandingData.xlsx
+++ b/StandingData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon\Documents\TAMUC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kendra\Box\VisualSearchStanding\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D02885-6E3B-421A-B280-57B9F473FCD8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12165" xr2:uid="{549C18B2-EF01-47DD-B9AA-6FC4B16CC290}"/>
   </bookViews>
   <sheets>
     <sheet name="Exp1RT" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
     <sheet name="Exp3RT" sheetId="5" r:id="rId5"/>
     <sheet name="Exp3Acc" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -112,7 +113,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -142,9 +143,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -160,49 +160,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>991209</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>95742</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="14097000" y="0"/>
-          <a:ext cx="4363059" cy="3524742"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -501,10 +458,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E94948C-4562-4EDD-B679-A57F130A885F}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
@@ -862,7 +819,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5302B17-1DD2-4688-A9AA-DE8A3355563C}">
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1227,7 +1184,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EA76C35-550A-4608-97E9-2E89D2051120}">
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2152,11 +2109,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20722D41-2F96-4C36-9CD4-5474E351513A}">
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2169,10 +2126,6 @@
     <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="27.140625" customWidth="1"/>
-    <col min="16" max="16" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -3074,96 +3027,18 @@
         <v>0.86666666699999995</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B34" s="1">
-        <f>AVERAGE(B2:B31)</f>
-        <v>0.97039395400000006</v>
-      </c>
-      <c r="C34" s="1">
-        <f t="shared" ref="C34:I34" si="0">AVERAGE(C2:C31)</f>
-        <v>0.93738491759999987</v>
-      </c>
-      <c r="D34" s="1">
-        <f t="shared" si="0"/>
-        <v>0.92253851236666706</v>
-      </c>
-      <c r="E34" s="1">
-        <f t="shared" si="0"/>
-        <v>0.83707885199999976</v>
-      </c>
-      <c r="F34" s="1">
-        <f t="shared" si="0"/>
-        <v>0.96995474626666678</v>
-      </c>
-      <c r="G34" s="1">
-        <f t="shared" si="0"/>
-        <v>0.95278775970000018</v>
-      </c>
-      <c r="H34" s="1">
-        <f t="shared" si="0"/>
-        <v>0.92968804926666648</v>
-      </c>
-      <c r="I34" s="1">
-        <f t="shared" si="0"/>
-        <v>0.87189627699999994</v>
-      </c>
-      <c r="N34" s="1"/>
-      <c r="O34" s="1"/>
-      <c r="P34" s="1"/>
-      <c r="Q34" s="1"/>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B35" s="1">
-        <f>STDEV(B2:B31)</f>
-        <v>3.4586401769067229E-2</v>
-      </c>
-      <c r="C35" s="1">
-        <f t="shared" ref="C35:I35" si="1">STDEV(C2:C31)</f>
-        <v>5.4577523376169966E-2</v>
-      </c>
-      <c r="D35" s="1">
-        <f t="shared" si="1"/>
-        <v>5.1317764533919771E-2</v>
-      </c>
-      <c r="E35" s="1">
-        <f t="shared" si="1"/>
-        <v>9.7170505318303457E-2</v>
-      </c>
-      <c r="F35" s="1">
-        <f t="shared" si="1"/>
-        <v>2.5190549475837199E-2</v>
-      </c>
-      <c r="G35" s="1">
-        <f t="shared" si="1"/>
-        <v>3.5456010844804674E-2</v>
-      </c>
-      <c r="H35" s="1">
-        <f t="shared" si="1"/>
-        <v>4.4196980928630038E-2</v>
-      </c>
-      <c r="I35" s="1">
-        <f t="shared" si="1"/>
-        <v>6.4109943621109514E-2</v>
-      </c>
-      <c r="N35" s="1"/>
-      <c r="O35" s="1"/>
-      <c r="P35" s="1"/>
-      <c r="Q35" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5B1EFC6-2A27-4F8B-BB76-1B7F4737E5BE}">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3477,7 +3352,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9876CC15-B4C4-46E7-94A3-7F4BE15F15C9}">
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>